<commit_message>
review changes to ms
</commit_message>
<xml_diff>
--- a/data/metadata/cruiseCbassMetadata.xlsx
+++ b/data/metadata/cruiseCbassMetadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rich/Documents/GradSchool/PhD/Projects/ApalGenomeSequencing_ApalCBASS_60minutes/Cruise/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rich/Documents/GradSchool/PhD/Projects/apalCBASS/data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B08EEE-E151-9A4B-A19A-D41566BD737A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D609F30B-66A9-D04E-9CAF-9C6BDF296206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29260" windowHeight="18880" xr2:uid="{CF0C6579-60F7-2442-89B2-BB19BF3EE6D6}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4477" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4475" uniqueCount="820">
   <si>
     <t>Date</t>
   </si>
@@ -2795,9 +2795,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2835,7 +2835,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2941,7 +2941,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3083,7 +3083,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3093,9 +3093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A57F98D-94E8-2847-B7A9-05D13C1D94F1}">
   <dimension ref="A1:AW205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM35" sqref="AM35"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9962,7 +9962,6 @@
         <v>231</v>
       </c>
       <c r="V86" s="21">
-        <f t="shared" ref="V86:V101" si="11">AJ86</f>
         <v>38538</v>
       </c>
       <c r="Y86" t="s">
@@ -10069,7 +10068,7 @@
         <v>31</v>
       </c>
       <c r="P87" t="str">
-        <f t="shared" ref="P87:P108" si="12">AL87</f>
+        <f t="shared" ref="P87:P108" si="11">AL87</f>
         <v>Upper Keys</v>
       </c>
       <c r="Q87" t="s">
@@ -10085,7 +10084,6 @@
         <v>238</v>
       </c>
       <c r="V87" s="21">
-        <f t="shared" si="11"/>
         <v>41920</v>
       </c>
       <c r="Y87" t="s">
@@ -10150,7 +10148,7 @@
         <v>Apal-69</v>
       </c>
       <c r="AV87" t="str">
-        <f t="shared" ref="AV87:AV100" si="13">RIGHT(AT87, 4)</f>
+        <f t="shared" ref="AV87:AV100" si="12">RIGHT(AT87, 4)</f>
         <v>ML16</v>
       </c>
       <c r="AW87" t="s">
@@ -10192,7 +10190,7 @@
         <v>31</v>
       </c>
       <c r="P88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q88" t="s">
@@ -10208,7 +10206,6 @@
         <v>244</v>
       </c>
       <c r="V88" s="21">
-        <f t="shared" si="11"/>
         <v>41907</v>
       </c>
       <c r="Y88" t="s">
@@ -10273,7 +10270,7 @@
         <v>Apal-67</v>
       </c>
       <c r="AV88" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> PK4</v>
       </c>
       <c r="AW88" t="s">
@@ -10315,7 +10312,7 @@
         <v>31</v>
       </c>
       <c r="P89" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q89" t="s">
@@ -10331,7 +10328,6 @@
         <v>250</v>
       </c>
       <c r="V89" s="21">
-        <f t="shared" si="11"/>
         <v>42473</v>
       </c>
       <c r="Y89" t="s">
@@ -10396,7 +10392,7 @@
         <v>Apal-2</v>
       </c>
       <c r="AV89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>pal2</v>
       </c>
       <c r="AW89" t="s">
@@ -10438,7 +10434,7 @@
         <v>31</v>
       </c>
       <c r="P90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q90" t="s">
@@ -10454,7 +10450,6 @@
         <v>256</v>
       </c>
       <c r="V90" s="21">
-        <f t="shared" si="11"/>
         <v>42473</v>
       </c>
       <c r="Y90" t="s">
@@ -10557,7 +10552,7 @@
         <v>31</v>
       </c>
       <c r="P91" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q91" t="s">
@@ -10573,7 +10568,6 @@
         <v>262</v>
       </c>
       <c r="V91" s="21">
-        <f t="shared" si="11"/>
         <v>42502</v>
       </c>
       <c r="Y91" t="s">
@@ -10676,7 +10670,7 @@
         <v>31</v>
       </c>
       <c r="P92" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Middle Keys</v>
       </c>
       <c r="Q92" t="s">
@@ -10692,7 +10686,6 @@
         <v>267</v>
       </c>
       <c r="V92" s="21">
-        <f t="shared" si="11"/>
         <v>42474</v>
       </c>
       <c r="Y92" t="s">
@@ -10795,7 +10788,7 @@
         <v>31</v>
       </c>
       <c r="P93" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q93" t="s">
@@ -10811,7 +10804,6 @@
         <v>273</v>
       </c>
       <c r="V93" s="21">
-        <f t="shared" si="11"/>
         <v>41494</v>
       </c>
       <c r="Y93" t="s">
@@ -10879,7 +10871,7 @@
         <v>Apal-39</v>
       </c>
       <c r="AV93" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>ELN1</v>
       </c>
       <c r="AW93" t="s">
@@ -10921,7 +10913,7 @@
         <v>31</v>
       </c>
       <c r="P94" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q94" t="s">
@@ -10937,7 +10929,6 @@
         <v>279</v>
       </c>
       <c r="V94" s="21">
-        <f t="shared" si="11"/>
         <v>41708</v>
       </c>
       <c r="Y94" t="s">
@@ -11005,7 +10996,7 @@
         <v>Apal-52</v>
       </c>
       <c r="AV94" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> SI5</v>
       </c>
       <c r="AW94" t="s">
@@ -11047,7 +11038,7 @@
         <v>31</v>
       </c>
       <c r="P95" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q95" t="s">
@@ -11063,7 +11054,6 @@
         <v>285</v>
       </c>
       <c r="V95" s="21">
-        <f t="shared" si="11"/>
         <v>41488</v>
       </c>
       <c r="Y95" t="s">
@@ -11131,7 +11121,7 @@
         <v>Apal-35</v>
       </c>
       <c r="AV95" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>NDR1</v>
       </c>
       <c r="AW95" t="s">
@@ -11173,7 +11163,7 @@
         <v>31</v>
       </c>
       <c r="P96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q96" t="s">
@@ -11189,7 +11179,6 @@
         <v>291</v>
       </c>
       <c r="V96" s="21">
-        <f t="shared" si="11"/>
         <v>44222</v>
       </c>
       <c r="Y96" t="s">
@@ -11257,7 +11246,7 @@
         <v>Apal-194</v>
       </c>
       <c r="AV96" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AW96" t="s">
@@ -11299,7 +11288,7 @@
         <v>31</v>
       </c>
       <c r="P97" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q97" t="s">
@@ -11315,7 +11304,6 @@
         <v>296</v>
       </c>
       <c r="V97" s="21">
-        <f t="shared" si="11"/>
         <v>41662</v>
       </c>
       <c r="Y97" t="s">
@@ -11383,7 +11371,7 @@
         <v>Apal-41</v>
       </c>
       <c r="AV97" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> ML6</v>
       </c>
       <c r="AW97" t="s">
@@ -11425,7 +11413,7 @@
         <v>31</v>
       </c>
       <c r="P98" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q98" t="s">
@@ -11441,7 +11429,6 @@
         <v>302</v>
       </c>
       <c r="V98" s="21">
-        <f t="shared" si="11"/>
         <v>41728</v>
       </c>
       <c r="Y98" t="s">
@@ -11509,7 +11496,7 @@
         <v>Apal-53</v>
       </c>
       <c r="AV98" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> FR1</v>
       </c>
       <c r="AW98" t="s">
@@ -11551,7 +11538,7 @@
         <v>31</v>
       </c>
       <c r="P99" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q99" t="s">
@@ -11567,7 +11554,6 @@
         <v>308</v>
       </c>
       <c r="V99" s="21">
-        <f t="shared" si="11"/>
         <v>41762</v>
       </c>
       <c r="Y99" t="s">
@@ -11635,7 +11621,7 @@
         <v>Apal-57</v>
       </c>
       <c r="AV99" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> TR1</v>
       </c>
       <c r="AW99" t="s">
@@ -11677,7 +11663,7 @@
         <v>31</v>
       </c>
       <c r="P100" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q100" t="s">
@@ -11693,7 +11679,6 @@
         <v>313</v>
       </c>
       <c r="V100" s="21">
-        <f t="shared" si="11"/>
         <v>41708</v>
       </c>
       <c r="Y100" t="s">
@@ -11761,7 +11746,7 @@
         <v>Apal-51</v>
       </c>
       <c r="AV100" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> ML3</v>
       </c>
       <c r="AW100" t="s">
@@ -11803,7 +11788,7 @@
         <v>31</v>
       </c>
       <c r="P101" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q101" t="s">
@@ -11819,7 +11804,6 @@
         <v>318</v>
       </c>
       <c r="V101" s="21">
-        <f t="shared" si="11"/>
         <v>43480</v>
       </c>
       <c r="Y101" t="s">
@@ -11880,7 +11864,7 @@
         <v>292</v>
       </c>
       <c r="AU101" t="str">
-        <f t="shared" ref="AU101:AU132" si="14">_xlfn.CONCAT("Apal-", N101)</f>
+        <f t="shared" ref="AU101:AU132" si="13">_xlfn.CONCAT("Apal-", N101)</f>
         <v>Apal-87</v>
       </c>
       <c r="AW101" t="s">
@@ -11939,7 +11923,7 @@
       <c r="U102" s="20">
         <v>12</v>
       </c>
-      <c r="V102" t="s">
+      <c r="V102" s="21" t="s">
         <v>646</v>
       </c>
       <c r="Y102" t="s">
@@ -11949,7 +11933,7 @@
         <v>174</v>
       </c>
       <c r="AU102" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-206</v>
       </c>
       <c r="AW102" t="s">
@@ -11991,7 +11975,7 @@
         <v>31</v>
       </c>
       <c r="P103" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q103" t="s">
@@ -12007,7 +11991,6 @@
         <v>323</v>
       </c>
       <c r="V103" s="21">
-        <f t="shared" ref="V103:V108" si="15">AJ103</f>
         <v>41914</v>
       </c>
       <c r="Y103" t="s">
@@ -12068,11 +12051,11 @@
         <v>324</v>
       </c>
       <c r="AU103" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-68</v>
       </c>
       <c r="AV103" t="str">
-        <f t="shared" ref="AV103" si="16">RIGHT(AT103, 4)</f>
+        <f t="shared" ref="AV103" si="14">RIGHT(AT103, 4)</f>
         <v>AAA3</v>
       </c>
       <c r="AW103" t="s">
@@ -12114,7 +12097,7 @@
         <v>31</v>
       </c>
       <c r="P104" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q104" t="s">
@@ -12130,7 +12113,6 @@
         <v>329</v>
       </c>
       <c r="V104" s="21">
-        <f t="shared" si="15"/>
         <v>43278</v>
       </c>
       <c r="Y104" t="s">
@@ -12194,7 +12176,7 @@
         <v>330</v>
       </c>
       <c r="AU104" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-29</v>
       </c>
       <c r="AW104" t="s">
@@ -12236,7 +12218,7 @@
         <v>31</v>
       </c>
       <c r="P105" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q105" t="s">
@@ -12252,7 +12234,6 @@
         <v>334</v>
       </c>
       <c r="V105" s="21">
-        <f t="shared" si="15"/>
         <v>42502</v>
       </c>
       <c r="Y105" t="s">
@@ -12316,7 +12297,7 @@
         <v>335</v>
       </c>
       <c r="AU105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-3</v>
       </c>
       <c r="AW105" t="s">
@@ -12358,7 +12339,7 @@
         <v>31</v>
       </c>
       <c r="P106" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Middle Keys</v>
       </c>
       <c r="Q106" t="s">
@@ -12374,7 +12355,6 @@
         <v>340</v>
       </c>
       <c r="V106" s="21">
-        <f t="shared" si="15"/>
         <v>42474</v>
       </c>
       <c r="Y106" t="s">
@@ -12435,7 +12415,7 @@
         <v>341</v>
       </c>
       <c r="AU106" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-9</v>
       </c>
       <c r="AW106" t="s">
@@ -12477,7 +12457,7 @@
         <v>31</v>
       </c>
       <c r="P107" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q107" t="s">
@@ -12493,7 +12473,6 @@
         <v>345</v>
       </c>
       <c r="V107" s="21">
-        <f t="shared" si="15"/>
         <v>42502</v>
       </c>
       <c r="Y107" t="s">
@@ -12554,7 +12533,7 @@
         <v>346</v>
       </c>
       <c r="AU107" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-24</v>
       </c>
       <c r="AW107" t="s">
@@ -12596,7 +12575,7 @@
         <v>31</v>
       </c>
       <c r="P108" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q108" t="s">
@@ -12612,7 +12591,6 @@
         <v>351</v>
       </c>
       <c r="V108" s="21">
-        <f t="shared" si="15"/>
         <v>42473</v>
       </c>
       <c r="Y108" t="s">
@@ -12673,7 +12651,7 @@
         <v>352</v>
       </c>
       <c r="AU108" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-5</v>
       </c>
       <c r="AW108" t="s">
@@ -12725,7 +12703,7 @@
         <v>206</v>
       </c>
       <c r="AU109" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-134</v>
       </c>
       <c r="AW109" t="s">
@@ -12777,7 +12755,7 @@
         <v>206</v>
       </c>
       <c r="AU110" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-8</v>
       </c>
       <c r="AW110" t="s">
@@ -12829,7 +12807,7 @@
         <v>206</v>
       </c>
       <c r="AU111" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-116</v>
       </c>
       <c r="AW111" t="s">
@@ -12881,7 +12859,7 @@
         <v>206</v>
       </c>
       <c r="AU112" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-114</v>
       </c>
       <c r="AW112" t="s">
@@ -12933,7 +12911,7 @@
         <v>206</v>
       </c>
       <c r="AU113" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-136</v>
       </c>
       <c r="AW113" t="s">
@@ -12985,7 +12963,7 @@
         <v>206</v>
       </c>
       <c r="AU114" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-21</v>
       </c>
       <c r="AW114" t="s">
@@ -13037,7 +13015,7 @@
         <v>206</v>
       </c>
       <c r="AU115" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-78</v>
       </c>
       <c r="AW115" t="s">
@@ -13089,7 +13067,7 @@
         <v>206</v>
       </c>
       <c r="AU116" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-104</v>
       </c>
       <c r="AW116" t="s">
@@ -13141,7 +13119,7 @@
         <v>206</v>
       </c>
       <c r="AU117" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-124</v>
       </c>
       <c r="AW117" t="s">
@@ -13185,6 +13163,7 @@
       <c r="Q118" t="s">
         <v>75</v>
       </c>
+      <c r="V118" s="21"/>
       <c r="X118" s="23" t="s">
         <v>707</v>
       </c>
@@ -13192,7 +13171,7 @@
         <v>206</v>
       </c>
       <c r="AU118" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-23</v>
       </c>
       <c r="AW118" t="s">
@@ -13234,7 +13213,7 @@
         <v>31</v>
       </c>
       <c r="P119" t="str">
-        <f t="shared" ref="P119:P173" si="17">AL119</f>
+        <f t="shared" ref="P119:P173" si="15">AL119</f>
         <v>Upper Keys</v>
       </c>
       <c r="Q119" t="s">
@@ -13250,7 +13229,6 @@
         <v>357</v>
       </c>
       <c r="V119" s="21">
-        <f t="shared" ref="V119:V129" si="18">AJ119</f>
         <v>41708</v>
       </c>
       <c r="Y119" t="s">
@@ -13311,11 +13289,11 @@
         <v>358</v>
       </c>
       <c r="AU119" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-49</v>
       </c>
       <c r="AV119" t="str">
-        <f t="shared" ref="AV119:AV173" si="19">RIGHT(AT119, 4)</f>
+        <f t="shared" ref="AV119:AV173" si="16">RIGHT(AT119, 4)</f>
         <v xml:space="preserve"> FR4</v>
       </c>
       <c r="AW119" t="s">
@@ -13357,7 +13335,7 @@
         <v>31</v>
       </c>
       <c r="P120" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q120" t="s">
@@ -13373,7 +13351,6 @@
         <v>362</v>
       </c>
       <c r="V120" s="21">
-        <f t="shared" si="18"/>
         <v>43357</v>
       </c>
       <c r="Y120" t="s">
@@ -13434,7 +13411,7 @@
         <v>292</v>
       </c>
       <c r="AU120" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-83</v>
       </c>
       <c r="AV120" t="s">
@@ -13479,7 +13456,7 @@
         <v>31</v>
       </c>
       <c r="P121" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q121" t="s">
@@ -13495,7 +13472,6 @@
         <v>367</v>
       </c>
       <c r="V121" s="21">
-        <f t="shared" si="18"/>
         <v>41762</v>
       </c>
       <c r="Y121" t="s">
@@ -13556,11 +13532,11 @@
         <v>368</v>
       </c>
       <c r="AU121" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-60</v>
       </c>
       <c r="AV121" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> TR5</v>
       </c>
       <c r="AW121" t="s">
@@ -13602,7 +13578,7 @@
         <v>31</v>
       </c>
       <c r="P122" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q122" t="s">
@@ -13618,7 +13594,6 @@
         <v>372</v>
       </c>
       <c r="V122" s="21">
-        <f t="shared" si="18"/>
         <v>41708</v>
       </c>
       <c r="Y122" t="s">
@@ -13679,11 +13654,11 @@
         <v>373</v>
       </c>
       <c r="AU122" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-47</v>
       </c>
       <c r="AV122" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> FR2</v>
       </c>
       <c r="AW122" t="s">
@@ -13725,7 +13700,7 @@
         <v>31</v>
       </c>
       <c r="P123" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q123" t="s">
@@ -13741,7 +13716,6 @@
         <v>377</v>
       </c>
       <c r="V123" s="21">
-        <f t="shared" si="18"/>
         <v>43357</v>
       </c>
       <c r="Y123" t="s">
@@ -13802,7 +13776,7 @@
         <v>292</v>
       </c>
       <c r="AU123" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-84</v>
       </c>
       <c r="AV123" t="s">
@@ -13847,7 +13821,7 @@
         <v>31</v>
       </c>
       <c r="P124" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q124" t="s">
@@ -13863,7 +13837,6 @@
         <v>381</v>
       </c>
       <c r="V124" s="21">
-        <f t="shared" si="18"/>
         <v>41662</v>
       </c>
       <c r="Y124" t="s">
@@ -13924,11 +13897,11 @@
         <v>382</v>
       </c>
       <c r="AU124" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-42</v>
       </c>
       <c r="AV124" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> SI1</v>
       </c>
       <c r="AW124" t="s">
@@ -13970,7 +13943,7 @@
         <v>31</v>
       </c>
       <c r="P125" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q125" t="s">
@@ -13986,7 +13959,6 @@
         <v>386</v>
       </c>
       <c r="V125" s="21">
-        <f t="shared" si="18"/>
         <v>41708</v>
       </c>
       <c r="Y125" t="s">
@@ -14047,11 +14019,11 @@
         <v>387</v>
       </c>
       <c r="AU125" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-50</v>
       </c>
       <c r="AV125" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> ML2</v>
       </c>
       <c r="AW125" t="s">
@@ -14093,7 +14065,7 @@
         <v>31</v>
       </c>
       <c r="P126" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q126" t="s">
@@ -14109,7 +14081,6 @@
         <v>391</v>
       </c>
       <c r="V126" s="21">
-        <f t="shared" si="18"/>
         <v>41488</v>
       </c>
       <c r="Y126" t="s">
@@ -14170,11 +14141,11 @@
         <v>392</v>
       </c>
       <c r="AU126" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-37</v>
       </c>
       <c r="AV126" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>AAA1</v>
       </c>
       <c r="AW126" t="s">
@@ -14216,7 +14187,7 @@
         <v>31</v>
       </c>
       <c r="P127" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q127" t="s">
@@ -14232,7 +14203,6 @@
         <v>396</v>
       </c>
       <c r="V127" s="21">
-        <f t="shared" si="18"/>
         <v>41708</v>
       </c>
       <c r="Y127" t="s">
@@ -14293,11 +14263,11 @@
         <v>373</v>
       </c>
       <c r="AU127" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-48</v>
       </c>
       <c r="AV127" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> FR2</v>
       </c>
       <c r="AW127" t="s">
@@ -14339,7 +14309,7 @@
         <v>31</v>
       </c>
       <c r="P128" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q128" t="s">
@@ -14355,7 +14325,6 @@
         <v>400</v>
       </c>
       <c r="V128" s="21">
-        <f t="shared" si="18"/>
         <v>43480</v>
       </c>
       <c r="Y128" t="s">
@@ -14416,11 +14385,11 @@
         <v>292</v>
       </c>
       <c r="AU128" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-86</v>
       </c>
       <c r="AV128" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AW128" t="s">
@@ -14462,7 +14431,7 @@
         <v>31</v>
       </c>
       <c r="P129" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q129" t="s">
@@ -14478,7 +14447,6 @@
         <v>404</v>
       </c>
       <c r="V129" s="21">
-        <f t="shared" si="18"/>
         <v>41291</v>
       </c>
       <c r="Y129" t="s">
@@ -14539,11 +14507,11 @@
         <v>405</v>
       </c>
       <c r="AU129" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-33</v>
       </c>
       <c r="AV129" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> EL1</v>
       </c>
       <c r="AW129" t="s">
@@ -14602,8 +14570,8 @@
       <c r="U130" s="20">
         <v>10</v>
       </c>
-      <c r="V130" t="s">
-        <v>646</v>
+      <c r="V130" s="21">
+        <v>44222</v>
       </c>
       <c r="Y130" t="s">
         <v>206</v>
@@ -14612,11 +14580,11 @@
         <v>210</v>
       </c>
       <c r="AU130" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-203</v>
       </c>
       <c r="AV130" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AW130" t="s">
@@ -14658,7 +14626,7 @@
         <v>31</v>
       </c>
       <c r="P131" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q131" t="s">
@@ -14674,7 +14642,6 @@
         <v>410</v>
       </c>
       <c r="V131" s="21">
-        <f t="shared" ref="V131:V150" si="20">AJ131</f>
         <v>41790</v>
       </c>
       <c r="Y131" t="s">
@@ -14735,11 +14702,11 @@
         <v>411</v>
       </c>
       <c r="AU131" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-63</v>
       </c>
       <c r="AV131" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> CF1</v>
       </c>
       <c r="AW131" t="s">
@@ -14781,7 +14748,7 @@
         <v>31</v>
       </c>
       <c r="P132" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q132" t="s">
@@ -14797,7 +14764,6 @@
         <v>416</v>
       </c>
       <c r="V132" s="21">
-        <f t="shared" si="20"/>
         <v>41743</v>
       </c>
       <c r="Y132" t="s">
@@ -14858,11 +14824,11 @@
         <v>417</v>
       </c>
       <c r="AU132" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>Apal-54</v>
       </c>
       <c r="AV132" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> GR2</v>
       </c>
       <c r="AW132" t="s">
@@ -14904,7 +14870,7 @@
         <v>31</v>
       </c>
       <c r="P133" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q133" t="s">
@@ -14920,7 +14886,6 @@
         <v>422</v>
       </c>
       <c r="V133" s="21">
-        <f t="shared" si="20"/>
         <v>41465</v>
       </c>
       <c r="Y133" t="s">
@@ -14984,11 +14949,11 @@
         <v>423</v>
       </c>
       <c r="AU133" t="str">
-        <f t="shared" ref="AU133:AU164" si="21">_xlfn.CONCAT("Apal-", N133)</f>
+        <f t="shared" ref="AU133:AU164" si="17">_xlfn.CONCAT("Apal-", N133)</f>
         <v>Apal-34</v>
       </c>
       <c r="AV133" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> PK2</v>
       </c>
       <c r="AW133" t="s">
@@ -15030,7 +14995,7 @@
         <v>31</v>
       </c>
       <c r="P134" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q134" t="s">
@@ -15046,7 +15011,6 @@
         <v>427</v>
       </c>
       <c r="V134" s="21">
-        <f t="shared" si="20"/>
         <v>44222</v>
       </c>
       <c r="Y134" t="s">
@@ -15107,11 +15071,11 @@
         <v>292</v>
       </c>
       <c r="AU134" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-90</v>
       </c>
       <c r="AV134" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AW134" t="s">
@@ -15153,7 +15117,7 @@
         <v>31</v>
       </c>
       <c r="P135" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q135" t="s">
@@ -15169,7 +15133,6 @@
         <v>431</v>
       </c>
       <c r="V135" s="21">
-        <f t="shared" si="20"/>
         <v>41745</v>
       </c>
       <c r="Y135" t="s">
@@ -15230,11 +15193,11 @@
         <v>432</v>
       </c>
       <c r="AU135" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-56</v>
       </c>
       <c r="AV135" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> GR3</v>
       </c>
       <c r="AW135" t="s">
@@ -15276,7 +15239,7 @@
         <v>31</v>
       </c>
       <c r="P136" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q136" t="s">
@@ -15292,7 +15255,6 @@
         <v>436</v>
       </c>
       <c r="V136" s="21">
-        <f t="shared" si="20"/>
         <v>42083</v>
       </c>
       <c r="Y136" t="s">
@@ -15353,11 +15315,11 @@
         <v>437</v>
       </c>
       <c r="AU136" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-72</v>
       </c>
       <c r="AV136" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> CN2</v>
       </c>
       <c r="AW136" t="s">
@@ -15399,7 +15361,7 @@
         <v>31</v>
       </c>
       <c r="P137" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q137" t="s">
@@ -15415,7 +15377,6 @@
         <v>441</v>
       </c>
       <c r="V137" s="21">
-        <f t="shared" si="20"/>
         <v>42083</v>
       </c>
       <c r="Y137" t="s">
@@ -15476,11 +15437,11 @@
         <v>442</v>
       </c>
       <c r="AU137" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-71</v>
       </c>
       <c r="AV137" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> CN3</v>
       </c>
       <c r="AW137" t="s">
@@ -15522,7 +15483,7 @@
         <v>31</v>
       </c>
       <c r="P138" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q138" t="s">
@@ -15538,7 +15499,6 @@
         <v>446</v>
       </c>
       <c r="V138" s="21">
-        <f t="shared" si="20"/>
         <v>42348</v>
       </c>
       <c r="Y138" t="s">
@@ -15599,11 +15559,11 @@
         <v>447</v>
       </c>
       <c r="AU138" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-79</v>
       </c>
       <c r="AV138" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> PK9</v>
       </c>
       <c r="AW138" t="s">
@@ -15645,7 +15605,7 @@
         <v>31</v>
       </c>
       <c r="P139" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q139" t="s">
@@ -15661,7 +15621,6 @@
         <v>451</v>
       </c>
       <c r="V139" s="21">
-        <f t="shared" si="20"/>
         <v>41488</v>
       </c>
       <c r="Y139" t="s">
@@ -15722,11 +15681,11 @@
         <v>452</v>
       </c>
       <c r="AU139" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-38</v>
       </c>
       <c r="AV139" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>AAA2</v>
       </c>
       <c r="AW139" t="s">
@@ -15768,7 +15727,7 @@
         <v>31</v>
       </c>
       <c r="P140" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q140" t="s">
@@ -15784,7 +15743,6 @@
         <v>456</v>
       </c>
       <c r="V140" s="21">
-        <f t="shared" si="20"/>
         <v>42339</v>
       </c>
       <c r="Y140" t="s">
@@ -15845,11 +15803,11 @@
         <v>457</v>
       </c>
       <c r="AU140" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-78</v>
       </c>
       <c r="AV140" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>PK10</v>
       </c>
       <c r="AW140" t="s">
@@ -15891,7 +15849,7 @@
         <v>31</v>
       </c>
       <c r="P141" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q141" t="s">
@@ -15907,7 +15865,6 @@
         <v>462</v>
       </c>
       <c r="V141" s="21">
-        <f t="shared" si="20"/>
         <v>41856</v>
       </c>
       <c r="Y141" t="s">
@@ -15968,11 +15925,11 @@
         <v>463</v>
       </c>
       <c r="AU141" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-66</v>
       </c>
       <c r="AV141" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> HS1</v>
       </c>
       <c r="AW141" t="s">
@@ -16014,7 +15971,7 @@
         <v>31</v>
       </c>
       <c r="P142" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q142" t="s">
@@ -16030,7 +15987,6 @@
         <v>467</v>
       </c>
       <c r="V142" s="21">
-        <f t="shared" si="20"/>
         <v>42125</v>
       </c>
       <c r="Y142" t="s">
@@ -16091,11 +16047,11 @@
         <v>468</v>
       </c>
       <c r="AU142" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-77</v>
       </c>
       <c r="AV142" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> CF9</v>
       </c>
       <c r="AW142" t="s">
@@ -16137,7 +16093,7 @@
         <v>31</v>
       </c>
       <c r="P143" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q143" t="s">
@@ -16153,7 +16109,6 @@
         <v>472</v>
       </c>
       <c r="V143" s="21">
-        <f t="shared" si="20"/>
         <v>41845</v>
       </c>
       <c r="Y143" t="s">
@@ -16214,11 +16169,11 @@
         <v>473</v>
       </c>
       <c r="AU143" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-28</v>
       </c>
       <c r="AV143" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>al28</v>
       </c>
       <c r="AW143" t="s">
@@ -16260,7 +16215,7 @@
         <v>31</v>
       </c>
       <c r="P144" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q144" t="s">
@@ -16276,7 +16231,6 @@
         <v>477</v>
       </c>
       <c r="V144" s="21">
-        <f t="shared" si="20"/>
         <v>42502</v>
       </c>
       <c r="Y144" t="s">
@@ -16337,11 +16291,11 @@
         <v>478</v>
       </c>
       <c r="AU144" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-21</v>
       </c>
       <c r="AV144" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>al21</v>
       </c>
       <c r="AW144" t="s">
@@ -16383,7 +16337,7 @@
         <v>31</v>
       </c>
       <c r="P145" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q145" t="s">
@@ -16399,7 +16353,6 @@
         <v>482</v>
       </c>
       <c r="V145" s="21">
-        <f t="shared" si="20"/>
         <v>41790</v>
       </c>
       <c r="Y145" t="s">
@@ -16457,11 +16410,11 @@
         <v>483</v>
       </c>
       <c r="AU145" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-65</v>
       </c>
       <c r="AV145" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> CF7</v>
       </c>
       <c r="AW145" t="s">
@@ -16503,7 +16456,7 @@
         <v>31</v>
       </c>
       <c r="P146" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q146" t="s">
@@ -16519,7 +16472,6 @@
         <v>487</v>
       </c>
       <c r="V146" s="21">
-        <f t="shared" si="20"/>
         <v>42473</v>
       </c>
       <c r="Y146" t="s">
@@ -16577,11 +16529,11 @@
         <v>488</v>
       </c>
       <c r="AU146" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-4</v>
       </c>
       <c r="AV146" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>pal4</v>
       </c>
       <c r="AW146" t="s">
@@ -16623,7 +16575,7 @@
         <v>31</v>
       </c>
       <c r="P147" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Middle Keys</v>
       </c>
       <c r="Q147" t="s">
@@ -16639,7 +16591,6 @@
         <v>492</v>
       </c>
       <c r="V147" s="21">
-        <f t="shared" si="20"/>
         <v>42474</v>
       </c>
       <c r="Y147" t="s">
@@ -16697,11 +16648,11 @@
         <v>493</v>
       </c>
       <c r="AU147" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-12</v>
       </c>
       <c r="AV147" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>al12</v>
       </c>
       <c r="AW147" t="s">
@@ -16743,7 +16694,7 @@
         <v>31</v>
       </c>
       <c r="P148" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q148" t="s">
@@ -16759,7 +16710,6 @@
         <v>498</v>
       </c>
       <c r="V148" s="21">
-        <f t="shared" si="20"/>
         <v>41160</v>
       </c>
       <c r="Y148" t="s">
@@ -16817,11 +16767,11 @@
         <v>437</v>
       </c>
       <c r="AU148" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-32</v>
       </c>
       <c r="AV148" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> CN2</v>
       </c>
       <c r="AW148" t="s">
@@ -16863,7 +16813,7 @@
         <v>31</v>
       </c>
       <c r="P149" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q149" t="s">
@@ -16879,7 +16829,6 @@
         <v>502</v>
       </c>
       <c r="V149" s="21">
-        <f t="shared" si="20"/>
         <v>44222</v>
       </c>
       <c r="Y149" t="s">
@@ -16937,11 +16886,11 @@
         <v>292</v>
       </c>
       <c r="AU149" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-156</v>
       </c>
       <c r="AV149" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AW149" t="s">
@@ -16983,7 +16932,7 @@
         <v>31</v>
       </c>
       <c r="P150" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q150" t="s">
@@ -16999,7 +16948,6 @@
         <v>506</v>
       </c>
       <c r="V150" s="21">
-        <f t="shared" si="20"/>
         <v>42473</v>
       </c>
       <c r="Y150" t="s">
@@ -17060,7 +17008,7 @@
         <v>507</v>
       </c>
       <c r="AU150" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-1</v>
       </c>
       <c r="AW150" t="s">
@@ -17102,7 +17050,7 @@
         <v>31</v>
       </c>
       <c r="P151" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q151" t="s">
@@ -17118,7 +17066,6 @@
         <v>512</v>
       </c>
       <c r="V151" s="21">
-        <f t="shared" ref="V151:V157" si="22">AJ151</f>
         <v>42502</v>
       </c>
       <c r="Y151" t="s">
@@ -17176,7 +17123,7 @@
         <v>513</v>
       </c>
       <c r="AU151" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-20</v>
       </c>
       <c r="AW151" t="s">
@@ -17218,7 +17165,7 @@
         <v>31</v>
       </c>
       <c r="P152" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q152" t="s">
@@ -17234,7 +17181,6 @@
         <v>517</v>
       </c>
       <c r="V152" s="21">
-        <f t="shared" si="22"/>
         <v>42125</v>
       </c>
       <c r="Y152" t="s">
@@ -17292,11 +17238,11 @@
         <v>518</v>
       </c>
       <c r="AU152" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-76</v>
       </c>
       <c r="AV152" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> CF8</v>
       </c>
       <c r="AW152" t="s">
@@ -17338,7 +17284,7 @@
         <v>31</v>
       </c>
       <c r="P153" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q153" t="s">
@@ -17354,7 +17300,6 @@
         <v>523</v>
       </c>
       <c r="V153" s="21">
-        <f t="shared" si="22"/>
         <v>41702</v>
       </c>
       <c r="Y153" t="s">
@@ -17412,11 +17357,11 @@
         <v>524</v>
       </c>
       <c r="AU153" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-45</v>
       </c>
       <c r="AV153" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> EL8</v>
       </c>
       <c r="AW153" t="s">
@@ -17458,7 +17403,7 @@
         <v>31</v>
       </c>
       <c r="P154" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q154" t="s">
@@ -17474,7 +17419,6 @@
         <v>528</v>
       </c>
       <c r="V154" s="21">
-        <f t="shared" si="22"/>
         <v>43482</v>
       </c>
       <c r="Y154" t="s">
@@ -17535,11 +17479,11 @@
         <v>292</v>
       </c>
       <c r="AU154" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-88</v>
       </c>
       <c r="AV154" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AW154" t="s">
@@ -17581,7 +17525,7 @@
         <v>31</v>
       </c>
       <c r="P155" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Middle Keys</v>
       </c>
       <c r="Q155" t="s">
@@ -17597,7 +17541,6 @@
         <v>533</v>
       </c>
       <c r="V155" s="21">
-        <f t="shared" si="22"/>
         <v>42474</v>
       </c>
       <c r="Y155" t="s">
@@ -17655,7 +17598,7 @@
         <v>534</v>
       </c>
       <c r="AU155" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-15</v>
       </c>
       <c r="AW155" t="s">
@@ -17697,7 +17640,7 @@
         <v>31</v>
       </c>
       <c r="P156" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q156" t="s">
@@ -17713,7 +17656,6 @@
         <v>539</v>
       </c>
       <c r="V156" s="21">
-        <f t="shared" si="22"/>
         <v>39939</v>
       </c>
       <c r="Y156" t="s">
@@ -17771,7 +17713,7 @@
         <v>540</v>
       </c>
       <c r="AU156" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-10</v>
       </c>
       <c r="AV156" t="s">
@@ -17816,7 +17758,7 @@
         <v>31</v>
       </c>
       <c r="P157" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q157" t="s">
@@ -17832,7 +17774,6 @@
         <v>544</v>
       </c>
       <c r="V157" s="21">
-        <f t="shared" si="22"/>
         <v>42110</v>
       </c>
       <c r="Y157" t="s">
@@ -17890,7 +17831,7 @@
         <v>545</v>
       </c>
       <c r="AU157" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-74</v>
       </c>
       <c r="AV157" t="s">
@@ -17952,18 +17893,18 @@
       <c r="U158" s="20">
         <v>5</v>
       </c>
-      <c r="V158" t="s">
-        <v>646</v>
+      <c r="V158" s="21">
+        <v>44222</v>
       </c>
       <c r="Y158" t="s">
         <v>206</v>
       </c>
       <c r="AU158" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-202</v>
       </c>
       <c r="AV158" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="AW158" t="s">
@@ -18005,7 +17946,7 @@
         <v>31</v>
       </c>
       <c r="P159" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q159" t="s">
@@ -18021,7 +17962,6 @@
         <v>512</v>
       </c>
       <c r="V159" s="21">
-        <f t="shared" ref="V159:V173" si="23">AJ159</f>
         <v>42502</v>
       </c>
       <c r="Y159" t="s">
@@ -18079,7 +18019,7 @@
         <v>513</v>
       </c>
       <c r="AU159" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-20</v>
       </c>
       <c r="AW159" t="s">
@@ -18121,7 +18061,7 @@
         <v>31</v>
       </c>
       <c r="P160" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Middle Keys</v>
       </c>
       <c r="Q160" t="s">
@@ -18137,7 +18077,6 @@
         <v>549</v>
       </c>
       <c r="V160" s="21">
-        <f t="shared" si="23"/>
         <v>42474</v>
       </c>
       <c r="Y160" t="s">
@@ -18198,7 +18137,7 @@
         <v>550</v>
       </c>
       <c r="AU160" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-14</v>
       </c>
       <c r="AW160" t="s">
@@ -18240,7 +18179,7 @@
         <v>31</v>
       </c>
       <c r="P161" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q161" t="s">
@@ -18256,7 +18195,6 @@
         <v>555</v>
       </c>
       <c r="V161" s="21">
-        <f t="shared" si="23"/>
         <v>41702</v>
       </c>
       <c r="Y161" t="s">
@@ -18314,11 +18252,11 @@
         <v>556</v>
       </c>
       <c r="AU161" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-43</v>
       </c>
       <c r="AV161" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> EL6</v>
       </c>
       <c r="AW161" t="s">
@@ -18360,7 +18298,7 @@
         <v>31</v>
       </c>
       <c r="P162" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q162" t="s">
@@ -18376,7 +18314,6 @@
         <v>561</v>
       </c>
       <c r="V162" s="21">
-        <f t="shared" si="23"/>
         <v>42348</v>
       </c>
       <c r="Y162" t="s">
@@ -18434,11 +18371,11 @@
         <v>562</v>
       </c>
       <c r="AU162" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-81</v>
       </c>
       <c r="AV162" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>Wat2</v>
       </c>
       <c r="AW162" t="s">
@@ -18480,7 +18417,7 @@
         <v>31</v>
       </c>
       <c r="P163" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q163" t="s">
@@ -18496,7 +18433,6 @@
         <v>567</v>
       </c>
       <c r="V163" s="21">
-        <f t="shared" si="23"/>
         <v>41762</v>
       </c>
       <c r="Y163" t="s">
@@ -18554,11 +18490,11 @@
         <v>568</v>
       </c>
       <c r="AU163" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-59</v>
       </c>
       <c r="AV163" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> TR3</v>
       </c>
       <c r="AW163" t="s">
@@ -18600,7 +18536,7 @@
         <v>31</v>
       </c>
       <c r="P164" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q164" t="s">
@@ -18616,7 +18552,6 @@
         <v>572</v>
       </c>
       <c r="V164" s="21">
-        <f t="shared" si="23"/>
         <v>39983</v>
       </c>
       <c r="Y164" t="s">
@@ -18674,11 +18609,11 @@
         <v>573</v>
       </c>
       <c r="AU164" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>Apal-30</v>
       </c>
       <c r="AV164" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> CN1</v>
       </c>
       <c r="AW164" t="s">
@@ -18720,7 +18655,7 @@
         <v>31</v>
       </c>
       <c r="P165" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q165" t="s">
@@ -18736,7 +18671,6 @@
         <v>578</v>
       </c>
       <c r="V165" s="21">
-        <f t="shared" si="23"/>
         <v>42502</v>
       </c>
       <c r="Y165" t="s">
@@ -18794,7 +18728,7 @@
         <v>579</v>
       </c>
       <c r="AU165" t="str">
-        <f t="shared" ref="AU165:AU173" si="24">_xlfn.CONCAT("Apal-", N165)</f>
+        <f t="shared" ref="AU165:AU173" si="18">_xlfn.CONCAT("Apal-", N165)</f>
         <v>Apal-18</v>
       </c>
       <c r="AW165" t="s">
@@ -18836,7 +18770,7 @@
         <v>31</v>
       </c>
       <c r="P166" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Lower Keys</v>
       </c>
       <c r="Q166" t="s">
@@ -18852,7 +18786,6 @@
         <v>583</v>
       </c>
       <c r="V166" s="21">
-        <f t="shared" si="23"/>
         <v>42502</v>
       </c>
       <c r="Y166" t="s">
@@ -18910,7 +18843,7 @@
         <v>584</v>
       </c>
       <c r="AU166" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="18"/>
         <v>Apal-23</v>
       </c>
       <c r="AW166" t="s">
@@ -18952,7 +18885,7 @@
         <v>31</v>
       </c>
       <c r="P167" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q167" t="s">
@@ -18968,7 +18901,6 @@
         <v>589</v>
       </c>
       <c r="V167" s="21">
-        <f t="shared" si="23"/>
         <v>42011</v>
       </c>
       <c r="Y167" t="s">
@@ -19026,11 +18958,11 @@
         <v>590</v>
       </c>
       <c r="AU167" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="18"/>
         <v>Apal-70</v>
       </c>
       <c r="AV167" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>Phil</v>
       </c>
       <c r="AW167" t="s">
@@ -19072,7 +19004,7 @@
         <v>31</v>
       </c>
       <c r="P168" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q168" t="s">
@@ -19088,7 +19020,6 @@
         <v>594</v>
       </c>
       <c r="V168" s="21">
-        <f t="shared" si="23"/>
         <v>42497</v>
       </c>
       <c r="Y168" t="s">
@@ -19149,7 +19080,7 @@
         <v>595</v>
       </c>
       <c r="AU168" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="18"/>
         <v>Apal-8</v>
       </c>
       <c r="AW168" t="s">
@@ -19191,7 +19122,7 @@
         <v>31</v>
       </c>
       <c r="P169" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q169" t="s">
@@ -19207,7 +19138,6 @@
         <v>599</v>
       </c>
       <c r="V169" s="21">
-        <f t="shared" si="23"/>
         <v>42348</v>
       </c>
       <c r="Y169" t="s">
@@ -19265,11 +19195,11 @@
         <v>600</v>
       </c>
       <c r="AU169" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="18"/>
         <v>Apal-82</v>
       </c>
       <c r="AV169" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>Wat3</v>
       </c>
       <c r="AW169" t="s">
@@ -19311,7 +19241,7 @@
         <v>31</v>
       </c>
       <c r="P170" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q170" t="s">
@@ -19327,7 +19257,6 @@
         <v>604</v>
       </c>
       <c r="V170" s="21">
-        <f t="shared" si="23"/>
         <v>42497</v>
       </c>
       <c r="Y170" t="s">
@@ -19388,7 +19317,7 @@
         <v>605</v>
       </c>
       <c r="AU170" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="18"/>
         <v>Apal-17</v>
       </c>
       <c r="AW170" t="s">
@@ -19430,7 +19359,7 @@
         <v>31</v>
       </c>
       <c r="P171" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q171" t="s">
@@ -19446,7 +19375,6 @@
         <v>609</v>
       </c>
       <c r="V171" s="21">
-        <f t="shared" si="23"/>
         <v>39974</v>
       </c>
       <c r="Y171" t="s">
@@ -19504,11 +19432,11 @@
         <v>610</v>
       </c>
       <c r="AU171" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="18"/>
         <v>Apal-27</v>
       </c>
       <c r="AV171" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> PK1</v>
       </c>
       <c r="AW171" t="s">
@@ -19550,7 +19478,7 @@
         <v>31</v>
       </c>
       <c r="P172" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q172" t="s">
@@ -19566,7 +19494,6 @@
         <v>313</v>
       </c>
       <c r="V172" s="21">
-        <f t="shared" si="23"/>
         <v>42497</v>
       </c>
       <c r="Y172" t="s">
@@ -19624,7 +19551,7 @@
         <v>613</v>
       </c>
       <c r="AU172" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="18"/>
         <v>Apal-16</v>
       </c>
       <c r="AW172" t="s">
@@ -19666,7 +19593,7 @@
         <v>31</v>
       </c>
       <c r="P173" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q173" t="s">
@@ -19682,7 +19609,6 @@
         <v>617</v>
       </c>
       <c r="V173" s="21">
-        <f t="shared" si="23"/>
         <v>39954</v>
       </c>
       <c r="Y173" t="s">
@@ -19740,11 +19666,11 @@
         <v>618</v>
       </c>
       <c r="AU173" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="18"/>
         <v>Apal-22</v>
       </c>
       <c r="AV173" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> ML1</v>
       </c>
       <c r="AW173" t="s">
@@ -19796,7 +19722,7 @@
         <v>210</v>
       </c>
       <c r="AU174" t="str">
-        <f t="shared" ref="AU174:AU201" si="25">_xlfn.CONCAT("Acer-", N174)</f>
+        <f t="shared" ref="AU174:AU201" si="19">_xlfn.CONCAT("Acer-", N174)</f>
         <v>Acer-27</v>
       </c>
       <c r="AW174" t="s">
@@ -19848,7 +19774,7 @@
         <v>210</v>
       </c>
       <c r="AU175" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-26</v>
       </c>
       <c r="AW175" t="s">
@@ -19890,26 +19816,25 @@
         <v>31</v>
       </c>
       <c r="P176" t="str">
-        <f t="shared" ref="P176:P202" si="26">AL176</f>
+        <f t="shared" ref="P176:P202" si="20">AL176</f>
         <v>Upper Keys</v>
       </c>
       <c r="Q176" t="s">
         <v>204</v>
       </c>
       <c r="R176" t="str">
-        <f t="shared" ref="R176:R202" si="27">AN176</f>
+        <f t="shared" ref="R176:R202" si="21">AN176</f>
         <v>Patch Reef inside Molasses Trench area</v>
       </c>
       <c r="S176" t="str">
-        <f t="shared" ref="S176:S202" si="28">AP176</f>
+        <f t="shared" ref="S176:S202" si="22">AP176</f>
         <v>25.00275°</v>
       </c>
       <c r="T176" t="str">
-        <f t="shared" ref="T176:T202" si="29">AQ176</f>
+        <f t="shared" ref="T176:T202" si="23">AQ176</f>
         <v>-80.422916°</v>
       </c>
       <c r="V176" s="21">
-        <f t="shared" ref="V176:V202" si="30">AJ176</f>
         <v>40269</v>
       </c>
       <c r="Y176" t="s">
@@ -19970,7 +19895,7 @@
         <v>785</v>
       </c>
       <c r="AU176" t="str">
-        <f t="shared" ref="AU176" si="31">_xlfn.CONCAT("Acer-", N176)</f>
+        <f t="shared" ref="AU176" si="24">_xlfn.CONCAT("Acer-", N176)</f>
         <v>Acer-61</v>
       </c>
       <c r="AW176" t="s">
@@ -20012,26 +19937,25 @@
         <v>31</v>
       </c>
       <c r="P177" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q177" t="s">
         <v>204</v>
       </c>
       <c r="R177" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Lower Matecumbe, Steph</v>
       </c>
       <c r="S177" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.80255°</v>
       </c>
       <c r="T177" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.6524°</v>
       </c>
       <c r="V177" s="21">
-        <f t="shared" si="30"/>
         <v>40576</v>
       </c>
       <c r="Y177" t="s">
@@ -20095,7 +20019,7 @@
         <v>758</v>
       </c>
       <c r="AU177" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-100</v>
       </c>
       <c r="AW177" t="s">
@@ -20137,26 +20061,25 @@
         <v>31</v>
       </c>
       <c r="P178" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q178" t="s">
         <v>204</v>
       </c>
       <c r="R178" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Patch Reef off Plantation Key (near 13)</v>
       </c>
       <c r="S178" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.9507°</v>
       </c>
       <c r="T178" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.490066°</v>
       </c>
       <c r="V178" s="21">
-        <f t="shared" si="30"/>
         <v>38730</v>
       </c>
       <c r="Y178" t="s">
@@ -20220,7 +20143,7 @@
         <v>765</v>
       </c>
       <c r="AU178" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-16</v>
       </c>
       <c r="AW178" t="s">
@@ -20262,26 +20185,25 @@
         <v>31</v>
       </c>
       <c r="P179" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q179" t="s">
         <v>204</v>
       </c>
       <c r="R179" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Cannon patch near Little Conch, Offshore Reef Edge</v>
       </c>
       <c r="S179" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.937533°</v>
       </c>
       <c r="T179" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.483533°</v>
       </c>
       <c r="V179" s="21">
-        <f t="shared" si="30"/>
         <v>39758</v>
       </c>
       <c r="Y179" t="s">
@@ -20345,7 +20267,7 @@
         <v>770</v>
       </c>
       <c r="AU179" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-44</v>
       </c>
       <c r="AW179" t="s">
@@ -20387,26 +20309,25 @@
         <v>31</v>
       </c>
       <c r="P180" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q180" t="s">
         <v>204</v>
       </c>
       <c r="R180" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Triple A patch reef</v>
       </c>
       <c r="S180" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.1687°</v>
       </c>
       <c r="T180" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.26795°</v>
       </c>
       <c r="V180" s="21">
-        <f t="shared" si="30"/>
         <v>41488</v>
       </c>
       <c r="Y180" t="s">
@@ -20470,7 +20391,7 @@
         <v>775</v>
       </c>
       <c r="AU180" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-107</v>
       </c>
       <c r="AW180" t="s">
@@ -20512,26 +20433,25 @@
         <v>31</v>
       </c>
       <c r="P181" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q181" t="s">
         <v>204</v>
       </c>
       <c r="R181" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Triangles Patch Reef</v>
       </c>
       <c r="S181" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.988466°</v>
       </c>
       <c r="T181" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.449883°</v>
       </c>
       <c r="V181" s="21">
-        <f t="shared" si="30"/>
         <v>38693</v>
       </c>
       <c r="Y181" t="s">
@@ -20595,7 +20515,7 @@
         <v>780</v>
       </c>
       <c r="AU181" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-11</v>
       </c>
       <c r="AW181" t="s">
@@ -20650,7 +20570,7 @@
         <v>210</v>
       </c>
       <c r="AU182" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-27</v>
       </c>
       <c r="AW182" t="s">
@@ -20705,7 +20625,7 @@
         <v>210</v>
       </c>
       <c r="AU183" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-26</v>
       </c>
       <c r="AW183" t="s">
@@ -20747,26 +20667,25 @@
         <v>31</v>
       </c>
       <c r="P184" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q184" t="s">
         <v>204</v>
       </c>
       <c r="R184" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Patch Reef inside Molasses Trench area</v>
       </c>
       <c r="S184" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.00275°</v>
       </c>
       <c r="T184" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.422916°</v>
       </c>
       <c r="V184" s="21">
-        <f t="shared" si="30"/>
         <v>40269</v>
       </c>
       <c r="Y184" t="s">
@@ -20830,7 +20749,7 @@
         <v>785</v>
       </c>
       <c r="AU184" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-61</v>
       </c>
       <c r="AW184" t="s">
@@ -20872,26 +20791,25 @@
         <v>31</v>
       </c>
       <c r="P185" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q185" t="s">
         <v>204</v>
       </c>
       <c r="R185" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Lower Matecumbe, Steph</v>
       </c>
       <c r="S185" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.80255°</v>
       </c>
       <c r="T185" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.6524°</v>
       </c>
       <c r="V185" s="21">
-        <f t="shared" si="30"/>
         <v>40576</v>
       </c>
       <c r="Y185" t="s">
@@ -20955,7 +20873,7 @@
         <v>758</v>
       </c>
       <c r="AU185" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-100</v>
       </c>
       <c r="AW185" t="s">
@@ -20997,26 +20915,25 @@
         <v>31</v>
       </c>
       <c r="P186" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q186" t="s">
         <v>204</v>
       </c>
       <c r="R186" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Patch Reef off Plantation Key (near 13)</v>
       </c>
       <c r="S186" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.9507°</v>
       </c>
       <c r="T186" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.490066°</v>
       </c>
       <c r="V186" s="21">
-        <f t="shared" si="30"/>
         <v>38730</v>
       </c>
       <c r="Y186" t="s">
@@ -21083,7 +21000,7 @@
         <v>765</v>
       </c>
       <c r="AU186" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-16</v>
       </c>
       <c r="AW186" t="s">
@@ -21125,26 +21042,25 @@
         <v>31</v>
       </c>
       <c r="P187" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q187" t="s">
         <v>204</v>
       </c>
       <c r="R187" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Cannon patch near Little Conch, Offshore Reef Edge</v>
       </c>
       <c r="S187" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.937533°</v>
       </c>
       <c r="T187" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.483533°</v>
       </c>
       <c r="V187" s="21">
-        <f t="shared" si="30"/>
         <v>39758</v>
       </c>
       <c r="Y187" t="s">
@@ -21211,7 +21127,7 @@
         <v>770</v>
       </c>
       <c r="AU187" t="str">
-        <f t="shared" ref="AU187:AU189" si="32">_xlfn.CONCAT("Acer-", N187)</f>
+        <f t="shared" ref="AU187:AU189" si="25">_xlfn.CONCAT("Acer-", N187)</f>
         <v>Acer-44</v>
       </c>
       <c r="AW187" t="s">
@@ -21253,26 +21169,25 @@
         <v>31</v>
       </c>
       <c r="P188" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q188" t="s">
         <v>204</v>
       </c>
       <c r="R188" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Triple A patch reef</v>
       </c>
       <c r="S188" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.1687°</v>
       </c>
       <c r="T188" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.26795°</v>
       </c>
       <c r="V188" s="21">
-        <f t="shared" si="30"/>
         <v>41488</v>
       </c>
       <c r="Y188" t="s">
@@ -21339,7 +21254,7 @@
         <v>775</v>
       </c>
       <c r="AU188" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>Acer-107</v>
       </c>
       <c r="AW188" t="s">
@@ -21381,26 +21296,25 @@
         <v>31</v>
       </c>
       <c r="P189" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q189" t="s">
         <v>204</v>
       </c>
       <c r="R189" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Triangles Patch Reef</v>
       </c>
       <c r="S189" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.988466°</v>
       </c>
       <c r="T189" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.449883°</v>
       </c>
       <c r="V189" s="21">
-        <f t="shared" si="30"/>
         <v>38693</v>
       </c>
       <c r="Y189" t="s">
@@ -21467,7 +21381,7 @@
         <v>780</v>
       </c>
       <c r="AU189" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="25"/>
         <v>Acer-11</v>
       </c>
       <c r="AW189" t="s">
@@ -21509,26 +21423,25 @@
         <v>31</v>
       </c>
       <c r="P190" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q190" t="s">
         <v>204</v>
       </c>
       <c r="R190" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Inside Little Conch, Possibly the same as U41</v>
       </c>
       <c r="S190" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.9463°</v>
       </c>
       <c r="T190" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.4708°</v>
       </c>
       <c r="V190" s="21">
-        <f t="shared" si="30"/>
         <v>43273</v>
       </c>
       <c r="Y190" t="s">
@@ -21589,7 +21502,7 @@
         <v>790</v>
       </c>
       <c r="AU190" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-125</v>
       </c>
       <c r="AW190" t="s">
@@ -21631,26 +21544,25 @@
         <v>31</v>
       </c>
       <c r="P191" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q191" t="s">
         <v>204</v>
       </c>
       <c r="R191" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Shallow patch reef near U10</v>
       </c>
       <c r="S191" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.0208°</v>
       </c>
       <c r="T191" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.40085°</v>
       </c>
       <c r="V191" s="21">
-        <f t="shared" si="30"/>
         <v>41920</v>
       </c>
       <c r="Y191" t="s">
@@ -21714,7 +21626,7 @@
         <v>799</v>
       </c>
       <c r="AU191" t="str">
-        <f t="shared" ref="AU191" si="33">_xlfn.CONCAT("Acer-", N191)</f>
+        <f t="shared" ref="AU191" si="26">_xlfn.CONCAT("Acer-", N191)</f>
         <v>Acer-130</v>
       </c>
       <c r="AW191" t="s">
@@ -21756,26 +21668,25 @@
         <v>31</v>
       </c>
       <c r="P192" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q192" t="s">
         <v>204</v>
       </c>
       <c r="R192" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Horseshoe Reef; fragment brought in by Bill Precht in June of 2009</v>
       </c>
       <c r="S192" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.13985°</v>
       </c>
       <c r="T192" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.294583°</v>
       </c>
       <c r="V192" s="21">
-        <f t="shared" si="30"/>
         <v>39992</v>
       </c>
       <c r="Y192" t="s">
@@ -21836,7 +21747,7 @@
         <v>794</v>
       </c>
       <c r="AU192" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-129</v>
       </c>
       <c r="AW192" t="s">
@@ -21878,26 +21789,25 @@
         <v>31</v>
       </c>
       <c r="P193" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q193" t="s">
         <v>204</v>
       </c>
       <c r="R193" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Higdons Reef</v>
       </c>
       <c r="S193" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.141716°</v>
       </c>
       <c r="T193" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.313683°</v>
       </c>
       <c r="V193" s="21">
-        <f t="shared" si="30"/>
         <v>43278</v>
       </c>
       <c r="Y193" t="s">
@@ -21958,7 +21868,7 @@
         <v>804</v>
       </c>
       <c r="AU193" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-124</v>
       </c>
       <c r="AW193" t="s">
@@ -22000,26 +21910,25 @@
         <v>31</v>
       </c>
       <c r="P194" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q194" t="s">
         <v>204</v>
       </c>
       <c r="R194" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Patch Reef inshore from Molasses Trench area</v>
       </c>
       <c r="S194" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.01075°</v>
       </c>
       <c r="T194" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.417°</v>
       </c>
       <c r="V194" s="21">
-        <f t="shared" si="30"/>
         <v>40461</v>
       </c>
       <c r="Y194" t="s">
@@ -22080,7 +21989,7 @@
         <v>809</v>
       </c>
       <c r="AU194" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-79</v>
       </c>
       <c r="AW194" t="s">
@@ -22122,26 +22031,25 @@
         <v>31</v>
       </c>
       <c r="P195" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q195" t="s">
         <v>204</v>
       </c>
       <c r="R195" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Patch Reef just off Triangle Marker off Tavernier</v>
       </c>
       <c r="S195" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.003066°</v>
       </c>
       <c r="T195" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.45085°</v>
       </c>
       <c r="V195" s="21">
-        <f t="shared" si="30"/>
         <v>39581</v>
       </c>
       <c r="Y195" t="s">
@@ -22202,7 +22110,7 @@
         <v>814</v>
       </c>
       <c r="AU195" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-41</v>
       </c>
       <c r="AW195" t="s">
@@ -22244,26 +22152,25 @@
         <v>31</v>
       </c>
       <c r="P196" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q196" t="s">
         <v>204</v>
       </c>
       <c r="R196" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Patch Reef inside Staghorn Nursery</v>
       </c>
       <c r="S196" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.983016°</v>
       </c>
       <c r="T196" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.44325°</v>
       </c>
       <c r="V196" s="21">
-        <f t="shared" si="30"/>
         <v>40460</v>
       </c>
       <c r="Y196" t="s">
@@ -22324,7 +22231,7 @@
         <v>819</v>
       </c>
       <c r="AU196" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-77</v>
       </c>
       <c r="AW196" t="s">
@@ -22366,26 +22273,25 @@
         <v>31</v>
       </c>
       <c r="P197" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q197" t="s">
         <v>204</v>
       </c>
       <c r="R197" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Inside Little Conch, Possibly the same as U41</v>
       </c>
       <c r="S197" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>24.9463°</v>
       </c>
       <c r="T197" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.4708°</v>
       </c>
       <c r="V197" s="21">
-        <f t="shared" si="30"/>
         <v>43273</v>
       </c>
       <c r="Y197" t="s">
@@ -22449,7 +22355,7 @@
         <v>790</v>
       </c>
       <c r="AU197" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-125</v>
       </c>
       <c r="AW197" t="s">
@@ -22491,26 +22397,25 @@
         <v>31</v>
       </c>
       <c r="P198" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q198" t="s">
         <v>204</v>
       </c>
       <c r="R198" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Shallow patch reef near U10</v>
       </c>
       <c r="S198" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.0208°</v>
       </c>
       <c r="T198" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.40085°</v>
       </c>
       <c r="V198" s="21">
-        <f t="shared" si="30"/>
         <v>41920</v>
       </c>
       <c r="Y198" t="s">
@@ -22577,7 +22482,7 @@
         <v>799</v>
       </c>
       <c r="AU198" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-130</v>
       </c>
       <c r="AW198" t="s">
@@ -22619,26 +22524,25 @@
         <v>31</v>
       </c>
       <c r="P199" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q199" t="s">
         <v>204</v>
       </c>
       <c r="R199" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Horseshoe Reef; fragment brought in by Bill Precht in June of 2009</v>
       </c>
       <c r="S199" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.13985°</v>
       </c>
       <c r="T199" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.294583°</v>
       </c>
       <c r="V199" s="21">
-        <f t="shared" si="30"/>
         <v>39992</v>
       </c>
       <c r="Y199" t="s">
@@ -22702,7 +22606,7 @@
         <v>794</v>
       </c>
       <c r="AU199" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-129</v>
       </c>
       <c r="AW199" t="s">
@@ -22744,26 +22648,25 @@
         <v>31</v>
       </c>
       <c r="P200" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q200" t="s">
         <v>204</v>
       </c>
       <c r="R200" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Higdons Reef</v>
       </c>
       <c r="S200" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.141716°</v>
       </c>
       <c r="T200" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.313683°</v>
       </c>
       <c r="V200" s="21">
-        <f t="shared" si="30"/>
         <v>43278</v>
       </c>
       <c r="Y200" t="s">
@@ -22827,7 +22730,7 @@
         <v>804</v>
       </c>
       <c r="AU200" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-124</v>
       </c>
       <c r="AW200" t="s">
@@ -22869,26 +22772,25 @@
         <v>31</v>
       </c>
       <c r="P201" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q201" t="s">
         <v>204</v>
       </c>
       <c r="R201" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Patch Reef inshore from Molasses Trench area</v>
       </c>
       <c r="S201" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.01075°</v>
       </c>
       <c r="T201" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.417°</v>
       </c>
       <c r="V201" s="21">
-        <f t="shared" si="30"/>
         <v>40461</v>
       </c>
       <c r="Y201" t="s">
@@ -22952,7 +22854,7 @@
         <v>809</v>
       </c>
       <c r="AU201" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="19"/>
         <v>Acer-79</v>
       </c>
       <c r="AW201" t="s">
@@ -22994,26 +22896,25 @@
         <v>31</v>
       </c>
       <c r="P202" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>Upper Keys</v>
       </c>
       <c r="Q202" t="s">
         <v>204</v>
       </c>
       <c r="R202" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>Patch Reef just off Triangle Marker off Tavernier</v>
       </c>
       <c r="S202" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="22"/>
         <v>25.003066°</v>
       </c>
       <c r="T202" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="23"/>
         <v>-80.45085°</v>
       </c>
       <c r="V202" s="21">
-        <f t="shared" si="30"/>
         <v>39581</v>
       </c>
       <c r="Y202" t="s">
@@ -23077,7 +22978,7 @@
         <v>814</v>
       </c>
       <c r="AU202" t="str">
-        <f t="shared" ref="AU202" si="34">_xlfn.CONCAT("Acer-", N202)</f>
+        <f t="shared" ref="AU202" si="27">_xlfn.CONCAT("Acer-", N202)</f>
         <v>Acer-41</v>
       </c>
       <c r="AW202" t="s">
@@ -23088,6 +22989,10 @@
       <c r="A203" s="1"/>
       <c r="C203" s="1"/>
       <c r="F203" s="2"/>
+      <c r="V203" s="21"/>
+    </row>
+    <row r="204" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="V204" s="21"/>
     </row>
     <row r="205" spans="1:49" x14ac:dyDescent="0.2">
       <c r="F205" s="2"/>

</xml_diff>